<commit_message>
Update: list of products, collections, and hosting servers.
</commit_message>
<xml_diff>
--- a/inst/external/modland_products.xlsx
+++ b/inst/external/modland_products.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\MODIS\inst\external\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\repo\MODIS\inst\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Version 4 - 5.5" sheetId="1" r:id="rId1"/>
@@ -615,7 +615,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -662,7 +662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -672,15 +672,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -701,7 +692,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -965,7 +956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
       <selection sqref="A1:E69"/>
     </sheetView>
   </sheetViews>
@@ -974,1176 +965,1176 @@
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="2">
         <v>5600</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="2">
         <v>500</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="2">
         <v>500</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="D5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="D6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="6">
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2">
         <v>500</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2">
         <v>500</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="6">
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2">
         <v>500</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2">
         <v>500</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="6">
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="2">
         <v>5600</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="E15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="6">
+      <c r="B16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="2">
         <v>5600</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="6">
+      <c r="B17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2">
         <v>5600</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="E17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="6">
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="2">
         <v>5600</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="E18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="2">
         <v>500</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="2">
         <v>500</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="E20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="2">
         <v>5600</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="2">
         <v>250</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="B24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="2">
         <v>250</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="E24" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="B25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E25" s="6" t="s">
+      <c r="D25" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="D26" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="D27" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="B28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="2">
         <v>5600</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="E28" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="B29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="2">
         <v>5600</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="E29" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="2">
         <v>5600</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="E30" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="B31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="2">
         <v>5600</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="6" t="s">
+      <c r="B32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="2">
         <v>500</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="E32" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="B33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="D33" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E34" s="6" t="s">
+      <c r="D34" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="6" t="s">
+      <c r="B35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="2">
         <v>5600</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="E35" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="6" t="s">
+      <c r="B36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="2">
         <v>5600</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="6" t="s">
+      <c r="B37" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="2">
         <v>250</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="E37" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" s="6" t="s">
+      <c r="B38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E38" s="6" t="s">
+      <c r="D38" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="6" t="s">
+      <c r="B39" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="D39" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="6" t="s">
+      <c r="B40" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D40" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="D40" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="6" t="s">
+      <c r="B41" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="D41" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="6" t="s">
+      <c r="B42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D42" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="D42" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43" s="6" t="s">
+      <c r="B43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D43" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E43" s="6" t="s">
+      <c r="D43" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" s="6" t="s">
+      <c r="B44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="2">
         <v>250</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="E44" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45" s="6" t="s">
+      <c r="B45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="2">
         <v>250</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E45" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" s="6" t="s">
+      <c r="B46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="2">
         <v>250</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" s="6" t="s">
+      <c r="B47" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="2">
         <v>500</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="E47" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C48" s="6" t="s">
+      <c r="B48" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="2">
         <v>5600</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="E48" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49" s="6" t="s">
+      <c r="B49" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D49" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="E49" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C50" s="6" t="s">
+      <c r="B50" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="2">
         <v>250</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="E50" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C51" s="6" t="s">
+      <c r="B51" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D51" s="2">
         <v>250</v>
       </c>
-      <c r="E51" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+      <c r="E51" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52" s="6" t="s">
+      <c r="B52" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D52" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E52" s="6" t="s">
+      <c r="D52" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B53" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C53" s="6" t="s">
+      <c r="B53" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D53" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+      <c r="D53" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B54" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C54" s="6" t="s">
+      <c r="B54" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D54" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+      <c r="D54" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C55" s="6" t="s">
+      <c r="B55" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D55" s="2">
         <v>5600</v>
       </c>
-      <c r="E55" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+      <c r="E55" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B56" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C56" s="6" t="s">
+      <c r="B56" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D56" s="2">
         <v>5600</v>
       </c>
-      <c r="E56" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+      <c r="E56" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B57" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C57" s="6" t="s">
+      <c r="B57" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D57" s="2">
         <v>5600</v>
       </c>
-      <c r="E57" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+      <c r="E57" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B58" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C58" s="6" t="s">
+      <c r="B58" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D58" s="2">
         <v>5600</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C59" s="6" t="s">
+      <c r="B59" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D59" s="2">
         <v>500</v>
       </c>
-      <c r="E59" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+      <c r="E59" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B60" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" s="6" t="s">
+      <c r="B60" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D60" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="D60" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C61" s="6" t="s">
+      <c r="B61" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D61" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E61" s="6" t="s">
+      <c r="D61" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B62" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C62" s="6" t="s">
+      <c r="B62" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D62" s="2">
         <v>5600</v>
       </c>
-      <c r="E62" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
+      <c r="E62" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B63" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C63" s="6" t="s">
+      <c r="B63" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D63" s="2">
         <v>5600</v>
       </c>
-      <c r="E63" s="6" t="s">
+      <c r="E63" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
+    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B64" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C64" s="6" t="s">
+      <c r="B64" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D64" s="2">
         <v>250</v>
       </c>
-      <c r="E64" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+      <c r="E64" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B65" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C65" s="6" t="s">
+      <c r="B65" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D65" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E65" s="6" t="s">
+      <c r="D65" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+    <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B66" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C66" s="6" t="s">
+      <c r="B66" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D66" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
+      <c r="D66" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B67" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" s="6" t="s">
+      <c r="B67" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D67" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
+      <c r="D67" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B68" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" s="6" t="s">
+      <c r="B68" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D68" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+      <c r="D68" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B69" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C69" s="6" t="s">
+      <c r="B69" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D69" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E69" s="6" t="s">
+      <c r="D69" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2226,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A154" sqref="A154"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2237,7 +2228,7 @@
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2254,7 +2245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>93</v>
       </c>
@@ -2271,7 +2262,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>94</v>
       </c>
@@ -2288,7 +2279,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
@@ -2305,7 +2296,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>97</v>
       </c>
@@ -2322,7 +2313,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -2356,7 +2347,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -2373,7 +2364,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -2390,7 +2381,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -2407,7 +2398,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -2424,7 +2415,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -2441,7 +2432,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -2458,7 +2449,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>98</v>
       </c>
@@ -2475,7 +2466,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>99</v>
       </c>
@@ -2492,7 +2483,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>100</v>
       </c>
@@ -2509,7 +2500,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>101</v>
       </c>
@@ -2526,7 +2517,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>102</v>
       </c>
@@ -2543,7 +2534,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>103</v>
       </c>
@@ -2560,7 +2551,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>104</v>
       </c>
@@ -2577,7 +2568,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>105</v>
       </c>
@@ -2594,7 +2585,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>106</v>
       </c>
@@ -2611,7 +2602,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>107</v>
       </c>
@@ -2628,7 +2619,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>108</v>
       </c>
@@ -2645,7 +2636,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>109</v>
       </c>
@@ -2662,7 +2653,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>110</v>
       </c>
@@ -2679,7 +2670,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>111</v>
       </c>
@@ -2696,7 +2687,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>112</v>
       </c>
@@ -2713,7 +2704,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>113</v>
       </c>
@@ -2730,7 +2721,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>114</v>
       </c>
@@ -2747,7 +2738,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>115</v>
       </c>
@@ -2764,7 +2755,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>116</v>
       </c>
@@ -2781,7 +2772,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>117</v>
       </c>
@@ -2798,7 +2789,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>118</v>
       </c>
@@ -2815,7 +2806,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>119</v>
       </c>
@@ -2832,7 +2823,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>120</v>
       </c>
@@ -2849,7 +2840,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>121</v>
       </c>
@@ -2866,7 +2857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>122</v>
       </c>
@@ -2883,7 +2874,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>123</v>
       </c>
@@ -2900,7 +2891,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>124</v>
       </c>
@@ -2917,7 +2908,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>125</v>
       </c>
@@ -2934,7 +2925,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>126</v>
       </c>
@@ -2951,7 +2942,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>127</v>
       </c>
@@ -2968,7 +2959,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>128</v>
       </c>
@@ -2985,7 +2976,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>129</v>
       </c>
@@ -3002,7 +2993,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>130</v>
       </c>
@@ -3019,7 +3010,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>131</v>
       </c>
@@ -3036,7 +3027,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>132</v>
       </c>
@@ -3053,7 +3044,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>133</v>
       </c>
@@ -3070,7 +3061,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>134</v>
       </c>
@@ -3087,7 +3078,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>135</v>
       </c>
@@ -3104,7 +3095,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>136</v>
       </c>
@@ -3121,7 +3112,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>137</v>
       </c>
@@ -3138,7 +3129,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>138</v>
       </c>
@@ -3155,7 +3146,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>139</v>
       </c>
@@ -3172,7 +3163,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>140</v>
       </c>
@@ -3189,7 +3180,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>141</v>
       </c>
@@ -3206,7 +3197,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>142</v>
       </c>
@@ -3223,7 +3214,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>143</v>
       </c>
@@ -3240,7 +3231,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>144</v>
       </c>
@@ -3257,7 +3248,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>145</v>
       </c>
@@ -3274,7 +3265,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>146</v>
       </c>
@@ -3291,7 +3282,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>147</v>
       </c>
@@ -3308,7 +3299,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>148</v>
       </c>
@@ -3325,7 +3316,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>149</v>
       </c>
@@ -3342,7 +3333,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>150</v>
       </c>
@@ -3359,7 +3350,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>151</v>
       </c>
@@ -3376,7 +3367,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>152</v>
       </c>
@@ -3393,7 +3384,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>153</v>
       </c>
@@ -3410,7 +3401,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>154</v>
       </c>
@@ -3427,7 +3418,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>155</v>
       </c>
@@ -3444,7 +3435,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>156</v>
       </c>
@@ -3461,7 +3452,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>157</v>
       </c>
@@ -3478,7 +3469,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>158</v>
       </c>
@@ -3495,7 +3486,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>159</v>
       </c>
@@ -3512,7 +3503,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>160</v>
       </c>
@@ -3529,7 +3520,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>161</v>
       </c>
@@ -3546,7 +3537,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>162</v>
       </c>
@@ -3563,7 +3554,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>163</v>
       </c>
@@ -3580,7 +3571,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>164</v>
       </c>
@@ -3597,7 +3588,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>165</v>
       </c>
@@ -3614,7 +3605,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>166</v>
       </c>
@@ -3631,7 +3622,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>31</v>
       </c>
@@ -3665,7 +3656,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>36</v>
       </c>
@@ -3682,7 +3673,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>38</v>
       </c>
@@ -3699,7 +3690,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>39</v>
       </c>
@@ -3716,7 +3707,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>40</v>
       </c>
@@ -3733,7 +3724,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>43</v>
       </c>
@@ -3750,7 +3741,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>44</v>
       </c>
@@ -3767,7 +3758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>45</v>
       </c>
@@ -3784,7 +3775,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>167</v>
       </c>
@@ -3801,7 +3792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>168</v>
       </c>
@@ -3818,7 +3809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>46</v>
       </c>
@@ -3835,7 +3826,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>47</v>
       </c>
@@ -3852,7 +3843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>48</v>
       </c>
@@ -3869,7 +3860,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>49</v>
       </c>
@@ -3886,7 +3877,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>51</v>
       </c>
@@ -3903,7 +3894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>52</v>
       </c>
@@ -3920,7 +3911,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>53</v>
       </c>
@@ -3937,7 +3928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>54</v>
       </c>
@@ -3954,7 +3945,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>55</v>
       </c>
@@ -3971,7 +3962,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>56</v>
       </c>
@@ -3988,7 +3979,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>57</v>
       </c>
@@ -4005,7 +3996,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>58</v>
       </c>
@@ -4022,7 +4013,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>170</v>
       </c>
@@ -4039,7 +4030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>171</v>
       </c>
@@ -4056,7 +4047,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>173</v>
       </c>
@@ -4073,7 +4064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>174</v>
       </c>
@@ -4090,7 +4081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>175</v>
       </c>
@@ -4107,7 +4098,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>176</v>
       </c>
@@ -4124,7 +4115,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>177</v>
       </c>
@@ -4141,7 +4132,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>178</v>
       </c>
@@ -4158,7 +4149,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>179</v>
       </c>
@@ -4175,7 +4166,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>66</v>
       </c>
@@ -4192,7 +4183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>180</v>
       </c>
@@ -4209,7 +4200,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>181</v>
       </c>
@@ -4226,7 +4217,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>69</v>
       </c>
@@ -4243,7 +4234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>71</v>
       </c>
@@ -4260,7 +4251,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>72</v>
       </c>
@@ -4277,7 +4268,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>73</v>
       </c>
@@ -4294,7 +4285,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>74</v>
       </c>
@@ -4311,7 +4302,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>75</v>
       </c>
@@ -4328,7 +4319,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>76</v>
       </c>
@@ -4345,7 +4336,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>77</v>
       </c>
@@ -4362,7 +4353,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>78</v>
       </c>
@@ -4379,7 +4370,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>182</v>
       </c>
@@ -4396,7 +4387,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>183</v>
       </c>
@@ -4413,7 +4404,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>79</v>
       </c>
@@ -4430,7 +4421,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>80</v>
       </c>
@@ -4447,7 +4438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>81</v>
       </c>
@@ -4464,7 +4455,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>82</v>
       </c>
@@ -4481,7 +4472,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>83</v>
       </c>
@@ -4498,7 +4489,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>84</v>
       </c>
@@ -4515,7 +4506,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>85</v>
       </c>
@@ -4532,7 +4523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>86</v>
       </c>
@@ -4549,7 +4540,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>87</v>
       </c>
@@ -4566,7 +4557,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>88</v>
       </c>
@@ -4583,7 +4574,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>89</v>
       </c>
@@ -4600,7 +4591,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>90</v>
       </c>
@@ -4617,7 +4608,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>184</v>
       </c>
@@ -4634,7 +4625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>185</v>
       </c>
@@ -4651,7 +4642,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>186</v>
       </c>
@@ -4668,7 +4659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>187</v>
       </c>
@@ -4685,7 +4676,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>188</v>
       </c>
@@ -4702,7 +4693,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>189</v>
       </c>

</xml_diff>

<commit_message>
Update: added MOD03 to products list; ignore Matteo's swath stuff.
</commit_message>
<xml_diff>
--- a/inst/external/modland_products.xlsx
+++ b/inst/external/modland_products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\florianD\Coding\repo\MODIS\inst\external\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\florianD\Coding\Git\MODIS\inst\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{81623B15-4380-4D23-A777-2DF81BA6D318}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F300FF-11C0-493D-998B-75737B726BC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version 4 - 5.5" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="189">
   <si>
     <t>Name</t>
   </si>
@@ -584,6 +584,15 @@
   </si>
   <si>
     <t>MOD44W</t>
+  </si>
+  <si>
+    <t>MOD03</t>
+  </si>
+  <si>
+    <t>Geolocation Fields</t>
+  </si>
+  <si>
+    <t>MYD03</t>
   </si>
 </sst>
 </file>
@@ -930,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1032,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E157"/>
+  <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2526,24 +2535,24 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>24</v>
+        <v>186</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="D88" s="2">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>25</v>
@@ -2552,15 +2561,15 @@
         <v>26</v>
       </c>
       <c r="D89" s="2">
-        <v>5600</v>
+        <v>500</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>25</v>
@@ -2568,8 +2577,8 @@
       <c r="C90" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>30</v>
+      <c r="D90" s="2">
+        <v>5600</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>28</v>
@@ -2577,7 +2586,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>25</v>
@@ -2585,8 +2594,8 @@
       <c r="C91" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D91" s="2">
-        <v>250</v>
+      <c r="D91" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>28</v>
@@ -2594,7 +2603,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>25</v>
@@ -2606,29 +2615,29 @@
         <v>250</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D93" s="2">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>25</v>
@@ -2640,12 +2649,12 @@
         <v>1000</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>25</v>
@@ -2657,12 +2666,12 @@
         <v>1000</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>25</v>
@@ -2671,15 +2680,15 @@
         <v>34</v>
       </c>
       <c r="D96" s="2">
-        <v>5600</v>
+        <v>1000</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>153</v>
+        <v>38</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>25</v>
@@ -2691,46 +2700,46 @@
         <v>5600</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>155</v>
+        <v>34</v>
       </c>
       <c r="D98" s="2">
         <v>5600</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>39</v>
+        <v>154</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>34</v>
+        <v>155</v>
       </c>
       <c r="D99" s="2">
         <v>5600</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>25</v>
@@ -2742,12 +2751,12 @@
         <v>5600</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>25</v>
@@ -2759,29 +2768,29 @@
         <v>5600</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D102" s="2">
-        <v>500</v>
+        <v>5600</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>25</v>
@@ -2790,7 +2799,7 @@
         <v>43</v>
       </c>
       <c r="D103" s="2">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>12</v>
@@ -2798,7 +2807,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>25</v>
@@ -2810,12 +2819,12 @@
         <v>1000</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>25</v>
@@ -2824,15 +2833,15 @@
         <v>43</v>
       </c>
       <c r="D105" s="2">
-        <v>5600</v>
+        <v>1000</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>25</v>
@@ -2844,12 +2853,12 @@
         <v>5600</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>25</v>
@@ -2858,32 +2867,32 @@
         <v>43</v>
       </c>
       <c r="D107" s="2">
-        <v>250</v>
+        <v>5600</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="D108" s="2">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>25</v>
@@ -2895,12 +2904,12 @@
         <v>1000</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>25</v>
@@ -2912,21 +2921,21 @@
         <v>1000</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>156</v>
+        <v>51</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D111" s="2">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>12</v>
@@ -2934,13 +2943,13 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>158</v>
+        <v>11</v>
       </c>
       <c r="D112" s="2">
         <v>500</v>
@@ -2951,7 +2960,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>25</v>
@@ -2963,63 +2972,63 @@
         <v>500</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="D114" s="2">
         <v>500</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D115" s="2">
         <v>500</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D116" s="2">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>25</v>
@@ -3036,7 +3045,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>25</v>
@@ -3053,7 +3062,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>25</v>
@@ -3065,35 +3074,35 @@
         <v>1000</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>56</v>
+        <v>165</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D120" s="2">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>185</v>
+        <v>56</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="D121" s="2">
         <v>250</v>
@@ -3104,24 +3113,24 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D122" s="2">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>25</v>
@@ -3138,41 +3147,41 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D124" s="2">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>59</v>
+        <v>188</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="D125" s="2">
-        <v>5600</v>
+        <v>1000</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>58</v>
@@ -3180,16 +3189,16 @@
       <c r="C126" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D126" s="2" t="s">
-        <v>30</v>
+      <c r="D126" s="2">
+        <v>500</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>58</v>
@@ -3198,7 +3207,7 @@
         <v>26</v>
       </c>
       <c r="D127" s="2">
-        <v>250</v>
+        <v>5600</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>28</v>
@@ -3206,7 +3215,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>58</v>
@@ -3214,50 +3223,50 @@
       <c r="C128" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D128" s="2">
-        <v>250</v>
+      <c r="D128" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D129" s="2">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D130" s="2">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>58</v>
@@ -3269,12 +3278,12 @@
         <v>1000</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>58</v>
@@ -3283,7 +3292,7 @@
         <v>34</v>
       </c>
       <c r="D132" s="2">
-        <v>5600</v>
+        <v>1000</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>28</v>
@@ -3291,7 +3300,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>168</v>
+        <v>65</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>58</v>
@@ -3300,7 +3309,7 @@
         <v>34</v>
       </c>
       <c r="D133" s="2">
-        <v>5600</v>
+        <v>1000</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>12</v>
@@ -3308,7 +3317,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>169</v>
+        <v>66</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>58</v>
@@ -3320,12 +3329,12 @@
         <v>5600</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>67</v>
+        <v>168</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>58</v>
@@ -3337,12 +3346,12 @@
         <v>5600</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>68</v>
+        <v>169</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>58</v>
@@ -3354,12 +3363,12 @@
         <v>5600</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>58</v>
@@ -3371,21 +3380,21 @@
         <v>5600</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D138" s="2">
-        <v>500</v>
+        <v>5600</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>12</v>
@@ -3393,24 +3402,24 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D139" s="2">
-        <v>1000</v>
+        <v>5600</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>58</v>
@@ -3419,15 +3428,15 @@
         <v>43</v>
       </c>
       <c r="D140" s="2">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>58</v>
@@ -3436,7 +3445,7 @@
         <v>43</v>
       </c>
       <c r="D141" s="2">
-        <v>5600</v>
+        <v>1000</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>12</v>
@@ -3444,7 +3453,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>58</v>
@@ -3453,7 +3462,7 @@
         <v>43</v>
       </c>
       <c r="D142" s="2">
-        <v>5600</v>
+        <v>1000</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>23</v>
@@ -3461,7 +3470,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>58</v>
@@ -3470,7 +3479,7 @@
         <v>43</v>
       </c>
       <c r="D143" s="2">
-        <v>250</v>
+        <v>5600</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>12</v>
@@ -3478,41 +3487,41 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="D144" s="2">
-        <v>1000</v>
+        <v>5600</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="D145" s="2">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>58</v>
@@ -3524,38 +3533,38 @@
         <v>1000</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>170</v>
+        <v>77</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D147" s="2">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>171</v>
+        <v>78</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>158</v>
+        <v>22</v>
       </c>
       <c r="D148" s="2">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>12</v>
@@ -3563,30 +3572,30 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>158</v>
+        <v>11</v>
       </c>
       <c r="D149" s="2">
         <v>500</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="D150" s="2">
         <v>500</v>
@@ -3596,59 +3605,59 @@
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>174</v>
-      </c>
-      <c r="B151" t="s">
+      <c r="A151" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B151" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C151" t="s">
-        <v>54</v>
-      </c>
-      <c r="D151">
+      <c r="C151" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D151" s="2">
         <v>500</v>
       </c>
-      <c r="E151" t="s">
+      <c r="E151" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>175</v>
-      </c>
-      <c r="B152" t="s">
+      <c r="A152" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C152" t="s">
-        <v>34</v>
-      </c>
-      <c r="D152">
-        <v>1000</v>
-      </c>
-      <c r="E152" t="s">
-        <v>28</v>
+      <c r="C152" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D152" s="2">
+        <v>500</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B153" t="s">
         <v>58</v>
       </c>
       <c r="C153" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D153">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E153" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B154" t="s">
         <v>58</v>
@@ -3665,7 +3674,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B155" t="s">
         <v>58</v>
@@ -3677,18 +3686,18 @@
         <v>1000</v>
       </c>
       <c r="E155" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B156" t="s">
         <v>58</v>
       </c>
       <c r="C156" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D156">
         <v>1000</v>
@@ -3699,18 +3708,52 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B157" t="s">
         <v>58</v>
       </c>
       <c r="C157" t="s">
+        <v>34</v>
+      </c>
+      <c r="D157">
+        <v>1000</v>
+      </c>
+      <c r="E157" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>179</v>
+      </c>
+      <c r="B158" t="s">
+        <v>58</v>
+      </c>
+      <c r="C158" t="s">
         <v>26</v>
       </c>
-      <c r="D157">
-        <v>1000</v>
-      </c>
-      <c r="E157" t="s">
+      <c r="D158">
+        <v>1000</v>
+      </c>
+      <c r="E158" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>180</v>
+      </c>
+      <c r="B159" t="s">
+        <v>58</v>
+      </c>
+      <c r="C159" t="s">
+        <v>26</v>
+      </c>
+      <c r="D159">
+        <v>1000</v>
+      </c>
+      <c r="E159" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>